<commit_message>
first day of testing
</commit_message>
<xml_diff>
--- a/test_matrix.xlsx
+++ b/test_matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\GitHub\pick-point\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A542E36C-E958-435A-ADA3-1AA0DD67D455}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D375EEB-E03A-49F5-B45C-D8C34BE991F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2100" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="70">
   <si>
     <t>Light Level</t>
   </si>
@@ -192,6 +192,75 @@
   </si>
   <si>
     <t>bird_food</t>
+  </si>
+  <si>
+    <t>Light Levels</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>All the way up</t>
+  </si>
+  <si>
+    <t>4 clicks down from all the way up</t>
+  </si>
+  <si>
+    <t>cat_ear (1, 0)</t>
+  </si>
+  <si>
+    <t>cat_food (1, 90)</t>
+  </si>
+  <si>
+    <t>cat_mouth (2, 0), bird_eyes (2, 90), dog_ear (4,0)</t>
+  </si>
+  <si>
+    <t>bird_mouth (3,0)</t>
+  </si>
+  <si>
+    <t>cat_food (1, 0)</t>
+  </si>
+  <si>
+    <t>dog_food (4,0)</t>
+  </si>
+  <si>
+    <t>dog_eyes (4, 0)</t>
+  </si>
+  <si>
+    <t>"Phantom Pick" occurred, tried picking a block that</t>
+  </si>
+  <si>
+    <t>was not present. Still completed all tasks.</t>
+  </si>
+  <si>
+    <t>dog_tail (1, 90)</t>
+  </si>
+  <si>
+    <t>bird_eyes (2, 0)</t>
+  </si>
+  <si>
+    <t>bird_mouth (1,0)</t>
+  </si>
+  <si>
+    <t>bird_mouth was knocked out when colliding with</t>
+  </si>
+  <si>
+    <t>camera stand. Rest of process completed.</t>
+  </si>
+  <si>
+    <t>bird_mouth (1, 90)</t>
+  </si>
+  <si>
+    <t>dog_mouth (4, 0)</t>
+  </si>
+  <si>
+    <t>bird_body (1,0)</t>
+  </si>
+  <si>
+    <t>bird_eyes (2,90), dog_mouth (3, 90)</t>
+  </si>
+  <si>
+    <t>bird_body (4, 90)</t>
   </si>
 </sst>
 </file>
@@ -417,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -440,6 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,6 +525,403 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295273</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>140143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00121333-5D2D-49AA-9451-2E0EF4E79D79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="28070" r="27485"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8178580" y="4794473"/>
+          <a:ext cx="1492688" cy="2533651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>321464</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>63707</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B52E932D-A153-4C90-AB55-43658AAE90A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="32164" r="25146"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8234654" y="6440986"/>
+          <a:ext cx="1454356" cy="2555085"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>316704</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>57261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>18815</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D710821F-5DFE-490D-9DA4-9275FE320BD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="34659" r="19318"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8064275" y="8245015"/>
+          <a:ext cx="1676054" cy="2445546"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>235742</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>123831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>129493</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EB54553-9335-4779-94ED-A5D3E043248B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="31642" r="25381"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8168427" y="9840971"/>
+          <a:ext cx="1529662" cy="2669382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171447</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>104780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>173076</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63D6828A-5EFE-4B69-AEDD-517F009F8294}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="36170" r="20745"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8124013" y="11516539"/>
+          <a:ext cx="1592296" cy="2771777"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>9529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>131968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82855F9E-FA3D-45DE-9EDF-A9A792C955BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="34546" r="27272"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8195764" y="13214058"/>
+          <a:ext cx="1455939" cy="2859881"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>126206</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>161928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60054471-3077-481B-B0D0-82D6651E9202}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="36923" r="20855"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8121254" y="14960205"/>
+          <a:ext cx="1628773" cy="2893219"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>47628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>4641</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED425DA5-ABFE-4B3A-91D3-8E07D4E1DCCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="36842" r="24671"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8208230" y="16680597"/>
+          <a:ext cx="1481013" cy="2886076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -720,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q5"/>
+  <dimension ref="B2:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,6 +1308,44 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="5"/>
     </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>278</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>389</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>451</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -852,8 +1357,1578 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDF08E8-6E84-41B4-B687-185D9C4267B7}">
   <dimension ref="B1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A94" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13">
+        <v>90</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>90</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>90</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>90</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="21">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>90</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="21">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3">
+        <v>90</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>90</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="21">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="4">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="22">
+        <v>0.17708333333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3">
+        <v>90</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3</v>
+      </c>
+      <c r="D41" s="3">
+        <v>90</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="18"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>90</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="18"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="21">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="4">
+        <v>4</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="G45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="21">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1</v>
+      </c>
+      <c r="D53" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" s="22">
+        <v>0.16111111111111112</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <v>90</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="2">
+        <v>3</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" s="18"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" s="18"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="21">
+        <v>4</v>
+      </c>
+      <c r="D61" s="3">
+        <v>90</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="4">
+        <v>2</v>
+      </c>
+      <c r="D62" s="5">
+        <v>90</v>
+      </c>
+      <c r="G62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" s="17"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="2">
+        <v>4</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G67" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="2">
+        <v>2</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="18"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="2">
+        <v>3</v>
+      </c>
+      <c r="D69" s="3">
+        <v>90</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69" s="18"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" s="21">
+        <v>4</v>
+      </c>
+      <c r="D70" s="3">
+        <v>90</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" s="4">
+        <v>1</v>
+      </c>
+      <c r="D71" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>28</v>
+      </c>
+      <c r="F74" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G75" s="22">
+        <v>0.15833333333333333</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="2">
+        <v>4</v>
+      </c>
+      <c r="D76" s="3">
+        <v>0</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G76" s="18"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="2">
+        <v>2</v>
+      </c>
+      <c r="D77" s="3">
+        <v>0</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C78" s="2">
+        <v>3</v>
+      </c>
+      <c r="D78" s="3">
+        <v>90</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G78" s="18"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" s="21">
+        <v>3</v>
+      </c>
+      <c r="D79" s="3">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="19"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="4">
+        <v>2</v>
+      </c>
+      <c r="D80" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0.16319444444444445</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1</v>
+      </c>
+      <c r="D85" s="3">
+        <v>0</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G85" s="18"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C86" s="2">
+        <v>4</v>
+      </c>
+      <c r="D86" s="3">
+        <v>0</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G86" s="18"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C87" s="2">
+        <v>4</v>
+      </c>
+      <c r="D87" s="3">
+        <v>90</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" s="21">
+        <v>2</v>
+      </c>
+      <c r="D88" s="3">
+        <v>0</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="19"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" s="4">
+        <v>2</v>
+      </c>
+      <c r="D89" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>28</v>
+      </c>
+      <c r="F92" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F93" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G93" s="17"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" s="2">
+        <v>4</v>
+      </c>
+      <c r="D94" s="3">
+        <v>90</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G94" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C95" s="2">
+        <v>1</v>
+      </c>
+      <c r="D95" s="3">
+        <v>0</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G95" s="18"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C96" s="2">
+        <v>2</v>
+      </c>
+      <c r="D96" s="3">
+        <v>90</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G96" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="21">
+        <v>3</v>
+      </c>
+      <c r="D97" s="3">
+        <v>90</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" s="19"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C98" s="4">
+        <v>4</v>
+      </c>
+      <c r="D98" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>28</v>
+      </c>
+      <c r="F101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F102" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" s="17"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" s="2">
+        <v>1</v>
+      </c>
+      <c r="D103" s="3">
+        <v>0</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G103" s="18"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" s="2">
+        <v>2</v>
+      </c>
+      <c r="D104" s="3">
+        <v>90</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G104" s="18"/>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C105" s="2">
+        <v>3</v>
+      </c>
+      <c r="D105" s="3">
+        <v>90</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G105" s="18"/>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" s="21">
+        <v>1</v>
+      </c>
+      <c r="D106" s="3">
+        <v>90</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" s="19"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" s="4">
+        <v>3</v>
+      </c>
+      <c r="D107" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>28</v>
+      </c>
+      <c r="F110" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F111" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G111" s="17"/>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C112" s="2">
+        <v>3</v>
+      </c>
+      <c r="D112" s="3">
+        <v>90</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G112" s="18"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C113" s="2">
+        <v>3</v>
+      </c>
+      <c r="D113" s="3">
+        <v>90</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G113" s="18"/>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" s="2">
+        <v>4</v>
+      </c>
+      <c r="D114" s="3">
+        <v>0</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G114" s="18"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115" s="21">
+        <v>2</v>
+      </c>
+      <c r="D115" s="3">
+        <v>0</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="19"/>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C116" s="4">
+        <v>3</v>
+      </c>
+      <c r="D116" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="F119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D120" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F120" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G120" s="17"/>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" s="2">
+        <v>1</v>
+      </c>
+      <c r="D121" s="3">
+        <v>0</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G121" s="18"/>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" s="2">
+        <v>3</v>
+      </c>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G122" s="18"/>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C123" s="2">
+        <v>1</v>
+      </c>
+      <c r="D123" s="3">
+        <v>90</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G123" s="18"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C124" s="21">
+        <v>2</v>
+      </c>
+      <c r="D124" s="3">
+        <v>90</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G124" s="19"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C125" s="4">
+        <v>4</v>
+      </c>
+      <c r="D125" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>28</v>
+      </c>
+      <c r="F128" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B129" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F129" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G129" s="17"/>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C130" s="2">
+        <v>4</v>
+      </c>
+      <c r="D130" s="3">
+        <v>0</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G130" s="18"/>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" s="2">
+        <v>1</v>
+      </c>
+      <c r="D131" s="3">
+        <v>90</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G131" s="18"/>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C132" s="2">
+        <v>2</v>
+      </c>
+      <c r="D132" s="3">
+        <v>90</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G132" s="18"/>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" s="21">
+        <v>4</v>
+      </c>
+      <c r="D133" s="3">
+        <v>90</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G133" s="19"/>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C134" s="4">
+        <v>3</v>
+      </c>
+      <c r="D134" s="5">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2C961E-68C5-4C1D-A494-9B4E0F76E987}">
+  <dimension ref="B1:G134"/>
+  <sheetViews>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91:G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="13">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>24</v>
@@ -914,7 +2989,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>27</v>
@@ -929,7 +3004,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>26</v>
@@ -944,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>25</v>
@@ -959,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -998,7 +3073,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>24</v>
@@ -1028,7 +3103,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>26</v>
@@ -1058,7 +3133,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -1102,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>24</v>
@@ -1132,7 +3207,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>26</v>
@@ -1261,7 +3336,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1315,7 +3390,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>27</v>
@@ -1345,7 +3420,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>25</v>
@@ -1360,7 +3435,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -1419,7 +3494,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>27</v>
@@ -1434,7 +3509,7 @@
         <v>2</v>
       </c>
       <c r="D51" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>26</v>
@@ -1464,7 +3539,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
@@ -1497,13 +3572,13 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="3">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>24</v>
@@ -1512,13 +3587,13 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C59" s="2">
         <v>3</v>
       </c>
       <c r="D59" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>27</v>
@@ -1527,10 +3602,10 @@
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C60" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D60" s="3">
         <v>0</v>
@@ -1542,13 +3617,13 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C61" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D61" s="3">
-        <v>-45</v>
+        <v>90</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>25</v>
@@ -1557,10 +3632,10 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C62" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="5">
         <v>90</v>
@@ -1602,7 +3677,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>24</v>
@@ -1662,7 +3737,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
@@ -1797,10 +3872,10 @@
         <v>45</v>
       </c>
       <c r="C85" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D85" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>24</v>
@@ -1845,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="D88" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>25</v>
@@ -1911,10 +3986,10 @@
         <v>34</v>
       </c>
       <c r="C95" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D95" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>27</v>
@@ -1944,7 +4019,7 @@
         <v>3</v>
       </c>
       <c r="D97" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>25</v>
@@ -1959,7 +4034,7 @@
         <v>4</v>
       </c>
       <c r="D98" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
@@ -2013,7 +4088,7 @@
         <v>2</v>
       </c>
       <c r="D104" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>27</v>
@@ -2097,7 +4172,7 @@
         <v>3</v>
       </c>
       <c r="D112" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>24</v>
@@ -2112,7 +4187,7 @@
         <v>3</v>
       </c>
       <c r="D113" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>27</v>
@@ -2127,7 +4202,7 @@
         <v>4</v>
       </c>
       <c r="D114" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>26</v>
@@ -2157,7 +4232,7 @@
         <v>3</v>
       </c>
       <c r="D116" s="5">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.25">
@@ -2226,7 +4301,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F123" s="6" t="s">
         <v>26</v>
@@ -2241,7 +4316,7 @@
         <v>2</v>
       </c>
       <c r="D124" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F124" s="7" t="s">
         <v>25</v>
@@ -2256,7 +4331,7 @@
         <v>4</v>
       </c>
       <c r="D125" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
@@ -2295,7 +4370,7 @@
         <v>4</v>
       </c>
       <c r="D130" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F130" s="6" t="s">
         <v>24</v>
@@ -2310,7 +4385,7 @@
         <v>1</v>
       </c>
       <c r="D131" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>27</v>
@@ -2355,21 +4430,20 @@
         <v>3</v>
       </c>
       <c r="D134" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2C961E-68C5-4C1D-A494-9B4E0F76E987}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FFF4D4-E83F-4E53-BA91-969A3DA88CE8}">
   <dimension ref="B1:G134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91:G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +4489,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="13">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>24</v>
@@ -2430,7 +4504,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>27</v>
@@ -2445,7 +4519,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>26</v>
@@ -2460,7 +4534,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>25</v>
@@ -2475,7 +4549,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -2514,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>24</v>
@@ -2544,7 +4618,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>26</v>
@@ -2574,7 +4648,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -2618,7 +4692,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>24</v>
@@ -2648,7 +4722,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>26</v>
@@ -2777,7 +4851,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -2831,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>27</v>
@@ -2861,7 +4935,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>25</v>
@@ -2876,7 +4950,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -2935,7 +5009,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>27</v>
@@ -2950,7 +5024,7 @@
         <v>2</v>
       </c>
       <c r="D51" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>26</v>
@@ -2980,7 +5054,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
@@ -3013,13 +5087,13 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="3">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>24</v>
@@ -3028,13 +5102,13 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C59" s="2">
         <v>3</v>
       </c>
       <c r="D59" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>27</v>
@@ -3043,10 +5117,10 @@
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C60" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D60" s="3">
         <v>0</v>
@@ -3058,13 +5132,13 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C61" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D61" s="3">
-        <v>-45</v>
+        <v>90</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>25</v>
@@ -3073,10 +5147,10 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C62" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="5">
         <v>90</v>
@@ -3118,7 +5192,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>24</v>
@@ -3178,7 +5252,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
@@ -3313,10 +5387,10 @@
         <v>45</v>
       </c>
       <c r="C85" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D85" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>24</v>
@@ -3361,7 +5435,7 @@
         <v>2</v>
       </c>
       <c r="D88" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>25</v>
@@ -3427,10 +5501,10 @@
         <v>34</v>
       </c>
       <c r="C95" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D95" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>27</v>
@@ -3460,7 +5534,7 @@
         <v>3</v>
       </c>
       <c r="D97" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>25</v>
@@ -3475,7 +5549,7 @@
         <v>4</v>
       </c>
       <c r="D98" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
@@ -3529,7 +5603,7 @@
         <v>2</v>
       </c>
       <c r="D104" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>27</v>
@@ -3613,7 +5687,7 @@
         <v>3</v>
       </c>
       <c r="D112" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>24</v>
@@ -3628,7 +5702,7 @@
         <v>3</v>
       </c>
       <c r="D113" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>27</v>
@@ -3643,7 +5717,7 @@
         <v>4</v>
       </c>
       <c r="D114" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>26</v>
@@ -3673,7 +5747,7 @@
         <v>3</v>
       </c>
       <c r="D116" s="5">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.25">
@@ -3742,7 +5816,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F123" s="6" t="s">
         <v>26</v>
@@ -3757,7 +5831,7 @@
         <v>2</v>
       </c>
       <c r="D124" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F124" s="7" t="s">
         <v>25</v>
@@ -3772,7 +5846,7 @@
         <v>4</v>
       </c>
       <c r="D125" s="5">
-        <v>-45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
@@ -3811,7 +5885,7 @@
         <v>4</v>
       </c>
       <c r="D130" s="3">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="F130" s="6" t="s">
         <v>24</v>
@@ -3826,7 +5900,7 @@
         <v>1</v>
       </c>
       <c r="D131" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>27</v>
@@ -3871,1522 +5945,7 @@
         <v>3</v>
       </c>
       <c r="D134" s="5">
-        <v>-90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FFF4D4-E83F-4E53-BA91-969A3DA88CE8}">
-  <dimension ref="B1:G134"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13">
-        <v>-90</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="2">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>45</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="4">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
-        <v>45</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3">
-        <v>90</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="2">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="21">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="19"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>45</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3">
-        <v>90</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="2">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3">
-        <v>45</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="21">
-        <v>3</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="2">
-        <v>4</v>
-      </c>
-      <c r="D31" s="3">
-        <v>90</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <v>90</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="21">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="19"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="4">
-        <v>4</v>
-      </c>
-      <c r="D35" s="5">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="17"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="2">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3">
-        <v>90</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="18"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="2">
-        <v>3</v>
-      </c>
-      <c r="D41" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="18"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="2">
-        <v>2</v>
-      </c>
-      <c r="D42" s="3">
-        <v>90</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="18"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="21">
-        <v>2</v>
-      </c>
-      <c r="D43" s="3">
-        <v>45</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="19"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="4">
-        <v>4</v>
-      </c>
-      <c r="D44" s="5">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G48" s="17"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" s="2">
-        <v>3</v>
-      </c>
-      <c r="D49" s="3">
-        <v>0</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G49" s="18"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="2">
-        <v>2</v>
-      </c>
-      <c r="D50" s="3">
-        <v>45</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" s="18"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="2">
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <v>45</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" s="18"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="21">
-        <v>1</v>
-      </c>
-      <c r="D52" s="3">
-        <v>0</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="19"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C53" s="4">
-        <v>1</v>
-      </c>
-      <c r="D53" s="5">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G57" s="17"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="2">
-        <v>1</v>
-      </c>
-      <c r="D58" s="3">
-        <v>45</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="18"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="2">
-        <v>3</v>
-      </c>
-      <c r="D59" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G59" s="18"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="2">
-        <v>3</v>
-      </c>
-      <c r="D60" s="3">
-        <v>0</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" s="18"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="21">
-        <v>3</v>
-      </c>
-      <c r="D61" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G61" s="19"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C62" s="4">
-        <v>3</v>
-      </c>
-      <c r="D62" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>28</v>
-      </c>
-      <c r="F65" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F66" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G66" s="17"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C67" s="2">
-        <v>4</v>
-      </c>
-      <c r="D67" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G67" s="18"/>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C68" s="2">
-        <v>2</v>
-      </c>
-      <c r="D68" s="3">
-        <v>0</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G68" s="18"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C69" s="2">
-        <v>3</v>
-      </c>
-      <c r="D69" s="3">
-        <v>90</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G69" s="18"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" s="21">
-        <v>4</v>
-      </c>
-      <c r="D70" s="3">
-        <v>90</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G70" s="19"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C71" s="4">
-        <v>1</v>
-      </c>
-      <c r="D71" s="5">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>28</v>
-      </c>
-      <c r="F74" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D75" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G75" s="17"/>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C76" s="2">
-        <v>4</v>
-      </c>
-      <c r="D76" s="3">
-        <v>0</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G76" s="18"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C77" s="2">
-        <v>2</v>
-      </c>
-      <c r="D77" s="3">
-        <v>0</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G77" s="18"/>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="2">
-        <v>3</v>
-      </c>
-      <c r="D78" s="3">
-        <v>90</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G78" s="18"/>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C79" s="21">
-        <v>3</v>
-      </c>
-      <c r="D79" s="3">
-        <v>0</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" s="19"/>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C80" s="4">
-        <v>2</v>
-      </c>
-      <c r="D80" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>28</v>
-      </c>
-      <c r="F83" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G84" s="17"/>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C85" s="2">
-        <v>4</v>
-      </c>
-      <c r="D85" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G85" s="18"/>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="2">
-        <v>4</v>
-      </c>
-      <c r="D86" s="3">
-        <v>0</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G86" s="18"/>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C87" s="2">
-        <v>4</v>
-      </c>
-      <c r="D87" s="3">
-        <v>90</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G87" s="18"/>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C88" s="21">
-        <v>2</v>
-      </c>
-      <c r="D88" s="3">
-        <v>45</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G88" s="19"/>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C89" s="4">
-        <v>2</v>
-      </c>
-      <c r="D89" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>28</v>
-      </c>
-      <c r="F92" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D93" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F93" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G93" s="17"/>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C94" s="2">
-        <v>4</v>
-      </c>
-      <c r="D94" s="3">
-        <v>90</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G94" s="18"/>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C95" s="2">
-        <v>4</v>
-      </c>
-      <c r="D95" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G95" s="18"/>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C96" s="2">
-        <v>2</v>
-      </c>
-      <c r="D96" s="3">
-        <v>90</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G96" s="18"/>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C97" s="21">
-        <v>3</v>
-      </c>
-      <c r="D97" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G97" s="19"/>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C98" s="4">
-        <v>4</v>
-      </c>
-      <c r="D98" s="5">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>28</v>
-      </c>
-      <c r="F101" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B102" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F102" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G102" s="17"/>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C103" s="2">
-        <v>1</v>
-      </c>
-      <c r="D103" s="3">
-        <v>0</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G103" s="18"/>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C104" s="2">
-        <v>2</v>
-      </c>
-      <c r="D104" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G104" s="18"/>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C105" s="2">
-        <v>3</v>
-      </c>
-      <c r="D105" s="3">
-        <v>90</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G105" s="18"/>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C106" s="21">
-        <v>1</v>
-      </c>
-      <c r="D106" s="3">
-        <v>90</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G106" s="19"/>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C107" s="4">
-        <v>3</v>
-      </c>
-      <c r="D107" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>28</v>
-      </c>
-      <c r="F110" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D111" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F111" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G111" s="17"/>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C112" s="2">
-        <v>3</v>
-      </c>
-      <c r="D112" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G112" s="18"/>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C113" s="2">
-        <v>3</v>
-      </c>
-      <c r="D113" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G113" s="18"/>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C114" s="2">
-        <v>4</v>
-      </c>
-      <c r="D114" s="3">
-        <v>45</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G114" s="18"/>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C115" s="21">
-        <v>2</v>
-      </c>
-      <c r="D115" s="3">
-        <v>0</v>
-      </c>
-      <c r="F115" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G115" s="19"/>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C116" s="4">
-        <v>3</v>
-      </c>
-      <c r="D116" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>28</v>
-      </c>
-      <c r="F119" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C120" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D120" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F120" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G120" s="17"/>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C121" s="2">
-        <v>1</v>
-      </c>
-      <c r="D121" s="3">
-        <v>0</v>
-      </c>
-      <c r="F121" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G121" s="18"/>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C122" s="2">
-        <v>3</v>
-      </c>
-      <c r="D122" s="3">
-        <v>0</v>
-      </c>
-      <c r="F122" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G122" s="18"/>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C123" s="2">
-        <v>1</v>
-      </c>
-      <c r="D123" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G123" s="18"/>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C124" s="21">
-        <v>2</v>
-      </c>
-      <c r="D124" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F124" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G124" s="19"/>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C125" s="4">
-        <v>4</v>
-      </c>
-      <c r="D125" s="5">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
-        <v>28</v>
-      </c>
-      <c r="F128" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B129" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D129" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F129" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G129" s="17"/>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B130" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C130" s="2">
-        <v>4</v>
-      </c>
-      <c r="D130" s="3">
-        <v>-45</v>
-      </c>
-      <c r="F130" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G130" s="18"/>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B131" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C131" s="2">
-        <v>1</v>
-      </c>
-      <c r="D131" s="3">
-        <v>-90</v>
-      </c>
-      <c r="F131" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G131" s="18"/>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B132" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C132" s="2">
-        <v>2</v>
-      </c>
-      <c r="D132" s="3">
-        <v>90</v>
-      </c>
-      <c r="F132" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G132" s="18"/>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B133" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C133" s="21">
-        <v>4</v>
-      </c>
-      <c r="D133" s="3">
-        <v>90</v>
-      </c>
-      <c r="F133" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G133" s="19"/>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C134" s="4">
-        <v>3</v>
-      </c>
-      <c r="D134" s="5">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>